<commit_message>
change job schedule assignment method
</commit_message>
<xml_diff>
--- a/extended/relaxation_result.xlsx
+++ b/extended/relaxation_result.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20391"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\extended-mip\extended\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D173E6-7EB0-4B5C-A9E6-5D9ED9623EBF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -48,15 +61,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -98,7 +119,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -130,9 +151,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -164,6 +203,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -339,14 +396,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1800.105886936188</v>
       </c>
@@ -357,18 +416,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1800.054173946381</v>
+        <v>1800.0541739463811</v>
       </c>
       <c r="B3">
-        <v>444.2375918328837</v>
+        <v>444.23759183288371</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update Gurobi result schedule
</commit_message>
<xml_diff>
--- a/extended/relaxation_result.xlsx
+++ b/extended/relaxation_result.xlsx
@@ -348,332 +348,332 @@
   <sheetData>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>85.5256679058075</v>
+        <v>922.356803894043</v>
       </c>
       <c r="B2">
-        <v>32.54400841837773</v>
+        <v>29.77652573723383</v>
       </c>
       <c r="C2">
-        <v>32.54400840452588</v>
+        <v>29.52512967424755</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>23.48927879333496</v>
+        <v>1800.029103040695</v>
       </c>
       <c r="B3">
-        <v>20.45309800704962</v>
+        <v>172.0132764561589</v>
       </c>
       <c r="C3">
-        <v>20.45309800704962</v>
+        <v>61.94300509923724</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>0.9587769508361816</v>
+        <v>1800.024947881699</v>
       </c>
       <c r="B4">
-        <v>0.04582549595877437</v>
+        <v>53.61333600293771</v>
       </c>
       <c r="C4">
-        <v>0.04582549595877437</v>
+        <v>37.9003799541165</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>22.15014290809631</v>
+        <v>1001.752865076065</v>
       </c>
       <c r="B5">
-        <v>19.88865929517008</v>
+        <v>97.66105119990154</v>
       </c>
       <c r="C5">
-        <v>19.88865929517008</v>
+        <v>97.38106729892448</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>126.6588878631592</v>
+        <v>1800.015377044678</v>
       </c>
       <c r="B6">
-        <v>75.24426760195806</v>
+        <v>78.94737691767912</v>
       </c>
       <c r="C6">
-        <v>74.81366744161249</v>
+        <v>50.74460587833157</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>254.9033350944519</v>
+        <v>1800.007972002029</v>
       </c>
       <c r="B7">
-        <v>81.68940334185828</v>
+        <v>63.27065289641369</v>
       </c>
       <c r="C7">
-        <v>80.91256333232953</v>
+        <v>40.83998661785475</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>32.02106904983521</v>
+        <v>1056.470659971237</v>
       </c>
       <c r="B8">
-        <v>56.11803076967256</v>
+        <v>75.16669942679187</v>
       </c>
       <c r="C8">
-        <v>56.11803076967237</v>
+        <v>74.47514465578878</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>168.3342840671539</v>
+        <v>1800.006425142288</v>
       </c>
       <c r="B9">
-        <v>133.5712952894656</v>
+        <v>93.47627693142671</v>
       </c>
       <c r="C9">
-        <v>133.5625047947028</v>
+        <v>48.04548705034094</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>300.8396279811859</v>
+        <v>1657.981845140457</v>
       </c>
       <c r="B10">
-        <v>27.15297998404554</v>
+        <v>62.13426192009212</v>
       </c>
       <c r="C10">
-        <v>26.92674838782147</v>
+        <v>61.66116771814921</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
-        <v>141.8619768619537</v>
+        <v>1800.014371871948</v>
       </c>
       <c r="B11">
-        <v>76.42825604958568</v>
+        <v>16.91760078202191</v>
       </c>
       <c r="C11">
-        <v>75.84706873389489</v>
+        <v>1.876862522905473</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <v>603.1673979759216</v>
+        <v>1800.008924007416</v>
       </c>
       <c r="B12">
-        <v>79.07287058066218</v>
+        <v>54.51425737646211</v>
       </c>
       <c r="C12">
-        <v>78.51550958484341</v>
+        <v>40.11320110412142</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>274.5086810588837</v>
+        <v>1800.025357961655</v>
       </c>
       <c r="B13">
-        <v>178.2739857306893</v>
+        <v>109.8504091104679</v>
       </c>
       <c r="C13">
-        <v>176.9257548553284</v>
+        <v>58.31575468341022</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>1800.013068914413</v>
+        <v>1800.035519123077</v>
       </c>
       <c r="B14">
-        <v>85.99211295581115</v>
+        <v>58.47945732726614</v>
       </c>
       <c r="C14">
-        <v>43.28671268299803</v>
+        <v>19.39498828940649</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15">
-        <v>1546.603281021118</v>
+        <v>18.12905406951904</v>
       </c>
       <c r="B15">
-        <v>70.00092104191864</v>
+        <v>18.11557489757924</v>
       </c>
       <c r="C15">
-        <v>69.37133938620744</v>
+        <v>18.11557489757924</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16">
-        <v>126.1900179386139</v>
+        <v>1800.016659021378</v>
       </c>
       <c r="B16">
-        <v>79.43375424769859</v>
+        <v>71.75748607984156</v>
       </c>
       <c r="C16">
-        <v>79.43375424769859</v>
+        <v>28.78186443296211</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17">
-        <v>315.7370040416718</v>
+        <v>1800.007781982422</v>
       </c>
       <c r="B17">
-        <v>30.20008796193154</v>
+        <v>31.06558919058114</v>
       </c>
       <c r="C17">
-        <v>29.94157365838477</v>
+        <v>15.35776508589702</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18">
-        <v>1800.002058982849</v>
+        <v>1800.012269020081</v>
       </c>
       <c r="B18">
-        <v>68.2818142719812</v>
+        <v>106.5975133184138</v>
       </c>
       <c r="C18">
-        <v>44.52116853429651</v>
+        <v>74.6320076280808</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19">
-        <v>20.13658499717712</v>
+        <v>1800.019261837006</v>
       </c>
       <c r="B19">
-        <v>38.5550860036815</v>
+        <v>25.630824372315</v>
       </c>
       <c r="C19">
-        <v>38.5550860036815</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20">
-        <v>59.02217197418213</v>
+        <v>1800.02040719986</v>
       </c>
       <c r="B20">
-        <v>65.74248225874116</v>
+        <v>84.21905247243454</v>
       </c>
       <c r="C20">
-        <v>65.54083971352895</v>
+        <v>62.99160145332882</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21">
-        <v>782.170832157135</v>
+        <v>1800.013839960098</v>
       </c>
       <c r="B21">
-        <v>79.73560421585647</v>
+        <v>31.38261863492477</v>
       </c>
       <c r="C21">
-        <v>78.96564985683115</v>
+        <v>0.08614865408327427</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22">
-        <v>56.89652681350708</v>
+        <v>1800.021936893463</v>
       </c>
       <c r="B22">
-        <v>43.3267519137376</v>
+        <v>35.46502725731479</v>
       </c>
       <c r="C22">
-        <v>43.25089588330579</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23">
-        <v>86.76934409141541</v>
+        <v>1800.019460916519</v>
       </c>
       <c r="B23">
-        <v>74.07053164694267</v>
+        <v>81.07479082057147</v>
       </c>
       <c r="C23">
-        <v>74.07053164694267</v>
+        <v>43.03001891869729</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24">
-        <v>397.7780270576477</v>
+        <v>1800.025895833969</v>
       </c>
       <c r="B24">
-        <v>70.86359644078442</v>
+        <v>94.85758957152964</v>
       </c>
       <c r="C24">
-        <v>70.86359644078442</v>
+        <v>49.12991088775048</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25">
-        <v>12.31067299842834</v>
+        <v>1800.017073869705</v>
       </c>
       <c r="B25">
-        <v>42.97606374053618</v>
+        <v>93.48909923890439</v>
       </c>
       <c r="C25">
-        <v>42.97606374053618</v>
+        <v>41.18696053878347</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26">
-        <v>3.425646066665649</v>
+        <v>1800.017382144928</v>
       </c>
       <c r="B26">
-        <v>7.583309881040416</v>
+        <v>163.9716926168116</v>
       </c>
       <c r="C26">
-        <v>7.583309881040416</v>
+        <v>73.65684718622603</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27">
-        <v>104.5154738426208</v>
+        <v>1800.011164903641</v>
       </c>
       <c r="B27">
-        <v>62.27242483311785</v>
+        <v>74.42324030702281</v>
       </c>
       <c r="C27">
-        <v>61.89009968538873</v>
+        <v>28.36626460955025</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28">
-        <v>866.9104850292206</v>
+        <v>1800.013070106506</v>
       </c>
       <c r="B28">
-        <v>92.48187990477909</v>
+        <v>54.46917897083244</v>
       </c>
       <c r="C28">
-        <v>91.79273334348891</v>
+        <v>14.04922060158905</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29">
-        <v>33.07910704612732</v>
+        <v>1800.044002056122</v>
       </c>
       <c r="B29">
-        <v>40.57051885274434</v>
+        <v>51.63601574645354</v>
       </c>
       <c r="C29">
-        <v>40.57051884420952</v>
+        <v>14.46231382738935</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30">
-        <v>1800.015331983566</v>
+        <v>1800.037311792374</v>
       </c>
       <c r="B30">
-        <v>203.4079182678003</v>
+        <v>95.9879650954289</v>
       </c>
       <c r="C30">
-        <v>133.9030080358974</v>
+        <v>27.69666180211224</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31">
-        <v>2016.865358114243</v>
+        <v>931.1446940898895</v>
       </c>
       <c r="B31">
-        <v>29.87704489762835</v>
+        <v>35.00571185716035</v>
       </c>
       <c r="C31">
-        <v>19.81348126662387</v>
+        <v>34.85394514358636</v>
       </c>
     </row>
   </sheetData>

</xml_diff>